<commit_message>
Fix the ieee14_wt3 models and add notes
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/ieee14_wt3n.xlsx
+++ b/andes/cases/ieee14/ieee14_wt3n.xlsx
@@ -7,29 +7,79 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Toggler" sheetId="1" r:id="rId1"/>
-    <sheet name="Bus" sheetId="2" r:id="rId2"/>
-    <sheet name="PQ" sheetId="3" r:id="rId3"/>
-    <sheet name="PV" sheetId="4" r:id="rId4"/>
-    <sheet name="Slack" sheetId="5" r:id="rId5"/>
-    <sheet name="Shunt" sheetId="6" r:id="rId6"/>
-    <sheet name="Line" sheetId="7" r:id="rId7"/>
-    <sheet name="Area" sheetId="8" r:id="rId8"/>
-    <sheet name="BusFreq" sheetId="9" r:id="rId9"/>
-    <sheet name="REGCA1" sheetId="10" r:id="rId10"/>
-    <sheet name="REECA1" sheetId="11" r:id="rId11"/>
-    <sheet name="REPCA1" sheetId="12" r:id="rId12"/>
-    <sheet name="WTDTA1" sheetId="13" r:id="rId13"/>
-    <sheet name="WTARA1" sheetId="14" r:id="rId14"/>
-    <sheet name="WTPTA1" sheetId="15" r:id="rId15"/>
-    <sheet name="WTTQA1" sheetId="16" r:id="rId16"/>
+    <sheet name="Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="Toggler" sheetId="2" r:id="rId2"/>
+    <sheet name="Bus" sheetId="3" r:id="rId3"/>
+    <sheet name="PQ" sheetId="4" r:id="rId4"/>
+    <sheet name="PV" sheetId="5" r:id="rId5"/>
+    <sheet name="Slack" sheetId="6" r:id="rId6"/>
+    <sheet name="Shunt" sheetId="7" r:id="rId7"/>
+    <sheet name="Line" sheetId="8" r:id="rId8"/>
+    <sheet name="Area" sheetId="9" r:id="rId9"/>
+    <sheet name="GENCLS" sheetId="10" r:id="rId10"/>
+    <sheet name="BusFreq" sheetId="11" r:id="rId11"/>
+    <sheet name="REGCA1" sheetId="12" r:id="rId12"/>
+    <sheet name="REECA1" sheetId="13" r:id="rId13"/>
+    <sheet name="REPCA1" sheetId="14" r:id="rId14"/>
+    <sheet name="WTDTA1" sheetId="15" r:id="rId15"/>
+    <sheet name="WTARA1" sheetId="16" r:id="rId16"/>
+    <sheet name="WTPTA1" sheetId="17" r:id="rId17"/>
+    <sheet name="WTTQA1" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="298">
+  <si>
+    <t>field</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>comment2</t>
+  </si>
+  <si>
+    <t>comment3</t>
+  </si>
+  <si>
+    <t>comment4</t>
+  </si>
+  <si>
+    <t>uid</t>
+  </si>
+  <si>
+    <t>File name</t>
+  </si>
+  <si>
+    <t>Created</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Note 2</t>
+  </si>
+  <si>
+    <t>ieee14_wt3n.xlsx</t>
+  </si>
+  <si>
+    <t>Hantao Cui</t>
+  </si>
+  <si>
+    <t>IEEE 14-buses system with all generators replaced by Type-3 generic wind generators.</t>
+  </si>
+  <si>
+    <t>A tiny synchronous generator (SG) is attached to Bus 1 to provide the implicit reference angle.</t>
+  </si>
+  <si>
+    <t>The impact of the SG is neglegible.</t>
+  </si>
   <si>
     <t>idx</t>
   </si>
@@ -49,9 +99,6 @@
     <t>t</t>
   </si>
   <si>
-    <t>uid</t>
-  </si>
-  <si>
     <t>Toggler_1</t>
   </si>
   <si>
@@ -319,6 +366,51 @@
     <t>AREA2</t>
   </si>
   <si>
+    <t>gen</t>
+  </si>
+  <si>
+    <t>coi</t>
+  </si>
+  <si>
+    <t>coi2</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>xl</t>
+  </si>
+  <si>
+    <t>xd1</t>
+  </si>
+  <si>
+    <t>kp</t>
+  </si>
+  <si>
+    <t>kw</t>
+  </si>
+  <si>
+    <t>S10</t>
+  </si>
+  <si>
+    <t>S12</t>
+  </si>
+  <si>
+    <t>gammap</t>
+  </si>
+  <si>
+    <t>gammaq</t>
+  </si>
+  <si>
+    <t>GENCLS_1</t>
+  </si>
+  <si>
+    <t>GENCLS 1</t>
+  </si>
+  <si>
     <t>Tf</t>
   </si>
   <si>
@@ -340,9 +432,6 @@
     <t>BusFreq_5</t>
   </si>
   <si>
-    <t>gen</t>
-  </si>
-  <si>
     <t>Tg</t>
   </si>
   <si>
@@ -355,6 +444,9 @@
     <t>Zerox</t>
   </si>
   <si>
+    <t>Lvplsw</t>
+  </si>
+  <si>
     <t>Lvpl1</t>
   </si>
   <si>
@@ -385,12 +477,6 @@
     <t>Accel</t>
   </si>
   <si>
-    <t>Iqmax</t>
-  </si>
-  <si>
-    <t>Iqmin</t>
-  </si>
-  <si>
     <t>REGCA1_1</t>
   </si>
   <si>
@@ -592,6 +678,9 @@
     <t>Fflag</t>
   </si>
   <si>
+    <t>PLflag</t>
+  </si>
+  <si>
     <t>Kp</t>
   </si>
   <si>
@@ -673,18 +762,21 @@
     <t>REPCA1_5</t>
   </si>
   <si>
-    <t>Ht</t>
-  </si>
-  <si>
-    <t>Hg</t>
+    <t>H</t>
+  </si>
+  <si>
+    <t>DAMP</t>
+  </si>
+  <si>
+    <t>Htfrac</t>
+  </si>
+  <si>
+    <t>Freq1</t>
   </si>
   <si>
     <t>Dshaft</t>
   </si>
   <si>
-    <t>Kshaft</t>
-  </si>
-  <si>
     <t>w0</t>
   </si>
   <si>
@@ -815,6 +907,9 @@
   </si>
   <si>
     <t>sp4</t>
+  </si>
+  <si>
+    <t>Tn</t>
   </si>
   <si>
     <t>WTTQA1_1</t>
@@ -1187,7 +1282,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1196,9 +1291,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1215,54 +1310,60 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3">
-        <v>1.1</v>
+      <c r="C6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1272,7 +1373,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y6"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1281,466 +1382,134 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>112</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>106</v>
+        <v>26</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>110</v>
+        <v>70</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="E2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="I2">
         <v>100</v>
       </c>
-      <c r="H2">
-        <v>0.1</v>
-      </c>
-      <c r="I2">
-        <v>999</v>
-      </c>
       <c r="J2">
-        <v>0.8</v>
+        <v>69</v>
       </c>
       <c r="K2">
-        <v>0.5</v>
+        <v>60</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>1.2</v>
+        <v>0.01</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>-1.2</v>
+        <v>0.302</v>
       </c>
       <c r="Q2">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>999</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>-999</v>
+        <v>1</v>
       </c>
       <c r="U2">
         <v>0</v>
       </c>
       <c r="V2">
-        <v>999</v>
-      </c>
-      <c r="W2">
-        <v>-999</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3">
-        <v>100</v>
-      </c>
-      <c r="H3">
-        <v>0.1</v>
-      </c>
-      <c r="I3">
-        <v>999</v>
-      </c>
-      <c r="J3">
-        <v>0.8</v>
-      </c>
-      <c r="K3">
-        <v>0.5</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>1.2</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
-        <v>0.4</v>
-      </c>
-      <c r="P3">
-        <v>-1.2</v>
-      </c>
-      <c r="Q3">
-        <v>0.1</v>
-      </c>
-      <c r="R3">
-        <v>0.7</v>
-      </c>
-      <c r="S3">
-        <v>999</v>
-      </c>
-      <c r="T3">
-        <v>-999</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
-      <c r="V3">
-        <v>999</v>
-      </c>
-      <c r="W3">
-        <v>-999</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>122</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4">
-        <v>100</v>
-      </c>
-      <c r="H4">
-        <v>0.1</v>
-      </c>
-      <c r="I4">
-        <v>999</v>
-      </c>
-      <c r="J4">
-        <v>0.8</v>
-      </c>
-      <c r="K4">
-        <v>0.5</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>1.2</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>0.4</v>
-      </c>
-      <c r="P4">
-        <v>-1.2</v>
-      </c>
-      <c r="Q4">
-        <v>0.1</v>
-      </c>
-      <c r="R4">
-        <v>0.7</v>
-      </c>
-      <c r="S4">
-        <v>999</v>
-      </c>
-      <c r="T4">
-        <v>-999</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>999</v>
-      </c>
-      <c r="W4">
-        <v>-999</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>123</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>100</v>
-      </c>
-      <c r="H5">
-        <v>0.1</v>
-      </c>
-      <c r="I5">
-        <v>999</v>
-      </c>
-      <c r="J5">
-        <v>0.8</v>
-      </c>
-      <c r="K5">
-        <v>0.5</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>1.2</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5">
-        <v>0.4</v>
-      </c>
-      <c r="P5">
-        <v>-1.2</v>
-      </c>
-      <c r="Q5">
-        <v>0.1</v>
-      </c>
-      <c r="R5">
-        <v>0.7</v>
-      </c>
-      <c r="S5">
-        <v>999</v>
-      </c>
-      <c r="T5">
-        <v>-999</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>999</v>
-      </c>
-      <c r="W5">
-        <v>-999</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>124</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>100</v>
-      </c>
-      <c r="H6">
-        <v>0.1</v>
-      </c>
-      <c r="I6">
-        <v>999</v>
-      </c>
-      <c r="J6">
-        <v>0.8</v>
-      </c>
-      <c r="K6">
-        <v>0.5</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>1.2</v>
-      </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="O6">
-        <v>0.4</v>
-      </c>
-      <c r="P6">
-        <v>-1.2</v>
-      </c>
-      <c r="Q6">
-        <v>0.1</v>
-      </c>
-      <c r="R6">
-        <v>0.7</v>
-      </c>
-      <c r="S6">
-        <v>999</v>
-      </c>
-      <c r="T6">
-        <v>-999</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-      <c r="V6">
-        <v>999</v>
-      </c>
-      <c r="W6">
-        <v>-999</v>
-      </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-      <c r="Y6">
-        <v>0.23</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1749,6 +1518,638 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>0.02</v>
+      </c>
+      <c r="G2">
+        <v>0.02</v>
+      </c>
+      <c r="H2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>0.02</v>
+      </c>
+      <c r="G3">
+        <v>0.02</v>
+      </c>
+      <c r="H3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>0.02</v>
+      </c>
+      <c r="G4">
+        <v>0.02</v>
+      </c>
+      <c r="H4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>0.02</v>
+      </c>
+      <c r="G5">
+        <v>0.02</v>
+      </c>
+      <c r="H5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0.02</v>
+      </c>
+      <c r="G6">
+        <v>0.02</v>
+      </c>
+      <c r="H6">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:X6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:24">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2">
+        <v>0.1</v>
+      </c>
+      <c r="I2">
+        <v>999</v>
+      </c>
+      <c r="J2">
+        <v>0.8</v>
+      </c>
+      <c r="K2">
+        <v>0.5</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1.2</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="P2">
+        <v>0.4</v>
+      </c>
+      <c r="Q2">
+        <v>-1.2</v>
+      </c>
+      <c r="R2">
+        <v>0.1</v>
+      </c>
+      <c r="S2">
+        <v>0.7</v>
+      </c>
+      <c r="T2">
+        <v>999</v>
+      </c>
+      <c r="U2">
+        <v>-999</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+      <c r="H3">
+        <v>0.1</v>
+      </c>
+      <c r="I3">
+        <v>999</v>
+      </c>
+      <c r="J3">
+        <v>0.8</v>
+      </c>
+      <c r="K3">
+        <v>0.5</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1.2</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>0.4</v>
+      </c>
+      <c r="Q3">
+        <v>-1.2</v>
+      </c>
+      <c r="R3">
+        <v>0.1</v>
+      </c>
+      <c r="S3">
+        <v>0.7</v>
+      </c>
+      <c r="T3">
+        <v>999</v>
+      </c>
+      <c r="U3">
+        <v>-999</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>0.1</v>
+      </c>
+      <c r="I4">
+        <v>999</v>
+      </c>
+      <c r="J4">
+        <v>0.8</v>
+      </c>
+      <c r="K4">
+        <v>0.5</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1.2</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>0.4</v>
+      </c>
+      <c r="Q4">
+        <v>-1.2</v>
+      </c>
+      <c r="R4">
+        <v>0.1</v>
+      </c>
+      <c r="S4">
+        <v>0.7</v>
+      </c>
+      <c r="T4">
+        <v>999</v>
+      </c>
+      <c r="U4">
+        <v>-999</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>0.1</v>
+      </c>
+      <c r="I5">
+        <v>999</v>
+      </c>
+      <c r="J5">
+        <v>0.8</v>
+      </c>
+      <c r="K5">
+        <v>0.5</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1.2</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>0.4</v>
+      </c>
+      <c r="Q5">
+        <v>-1.2</v>
+      </c>
+      <c r="R5">
+        <v>0.1</v>
+      </c>
+      <c r="S5">
+        <v>0.7</v>
+      </c>
+      <c r="T5">
+        <v>999</v>
+      </c>
+      <c r="U5">
+        <v>-999</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <v>0.1</v>
+      </c>
+      <c r="I6">
+        <v>999</v>
+      </c>
+      <c r="J6">
+        <v>0.8</v>
+      </c>
+      <c r="K6">
+        <v>0.5</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1.2</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>0.4</v>
+      </c>
+      <c r="Q6">
+        <v>-1.2</v>
+      </c>
+      <c r="R6">
+        <v>0.1</v>
+      </c>
+      <c r="S6">
+        <v>0.7</v>
+      </c>
+      <c r="T6">
+        <v>999</v>
+      </c>
+      <c r="U6">
+        <v>-999</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BD6"/>
   <sheetViews>
@@ -1761,172 +2162,172 @@
   <sheetData>
     <row r="1" spans="1:56">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>125</v>
+        <v>153</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>127</v>
+        <v>155</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>129</v>
+        <v>157</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>137</v>
+        <v>165</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>140</v>
+        <v>168</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>144</v>
+        <v>172</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>148</v>
+        <v>176</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>149</v>
+        <v>177</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>150</v>
+        <v>178</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>151</v>
+        <v>179</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>153</v>
+        <v>181</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>156</v>
+        <v>184</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>157</v>
+        <v>185</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>158</v>
+        <v>186</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>159</v>
+        <v>187</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>160</v>
+        <v>188</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>161</v>
+        <v>189</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>163</v>
+        <v>191</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>164</v>
+        <v>192</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>165</v>
+        <v>193</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>166</v>
+        <v>194</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>167</v>
+        <v>195</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>168</v>
+        <v>196</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>169</v>
+        <v>197</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>170</v>
+        <v>198</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>171</v>
+        <v>199</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>172</v>
+        <v>200</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>173</v>
+        <v>201</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>174</v>
+        <v>202</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>175</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:56">
@@ -1934,16 +2335,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
       <c r="E2" t="s">
-        <v>120</v>
+        <v>148</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -2101,16 +2502,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
       <c r="E3" t="s">
-        <v>121</v>
+        <v>149</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -2268,16 +2669,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>178</v>
+        <v>206</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>178</v>
+        <v>206</v>
       </c>
       <c r="E4" t="s">
-        <v>122</v>
+        <v>150</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -2435,16 +2836,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
       <c r="E5" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
       <c r="G5">
         <v>0</v>
@@ -2602,16 +3003,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>180</v>
+        <v>208</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>180</v>
+        <v>208</v>
       </c>
       <c r="E6" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -2769,9 +3170,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AL6"/>
+  <dimension ref="A1:AM6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2780,143 +3181,146 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:39">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>181</v>
+        <v>209</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>182</v>
+        <v>210</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>183</v>
+        <v>211</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>184</v>
+        <v>212</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>185</v>
+        <v>213</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>186</v>
+        <v>214</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>113</v>
+        <v>215</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>187</v>
+        <v>143</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>188</v>
+        <v>216</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>189</v>
+        <v>217</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>190</v>
+        <v>218</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>191</v>
+        <v>219</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>192</v>
+        <v>220</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>193</v>
+        <v>221</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>194</v>
+        <v>222</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>195</v>
+        <v>223</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>196</v>
+        <v>224</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>134</v>
+        <v>225</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>135</v>
+        <v>162</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>198</v>
+        <v>226</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>199</v>
+        <v>227</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>200</v>
+        <v>228</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>143</v>
+        <v>229</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
       <c r="AG1" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E2" t="s">
         <v>204</v>
       </c>
-      <c r="AH1" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="2" spans="1:38">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>209</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>209</v>
-      </c>
-      <c r="E2" t="s">
-        <v>176</v>
-      </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="H2" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -2928,102 +3332,105 @@
         <v>0</v>
       </c>
       <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
         <v>0.02</v>
       </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
       <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
         <v>0.1</v>
       </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
       <c r="P2">
         <v>1</v>
       </c>
       <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2">
         <v>0.8</v>
       </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
       <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2">
         <v>999</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>-999</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>-0.02</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>0.02</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>999</v>
       </c>
-      <c r="Z2">
+      <c r="AA2">
         <v>-999</v>
       </c>
-      <c r="AA2">
-        <v>1</v>
-      </c>
       <c r="AB2">
+        <v>1</v>
+      </c>
+      <c r="AC2">
         <v>0.1</v>
       </c>
-      <c r="AC2">
+      <c r="AD2">
         <v>0.02</v>
       </c>
-      <c r="AD2">
+      <c r="AE2">
         <v>-0.01</v>
       </c>
-      <c r="AE2">
+      <c r="AF2">
         <v>0.01</v>
       </c>
-      <c r="AF2">
+      <c r="AG2">
         <v>0.05</v>
       </c>
-      <c r="AG2">
+      <c r="AH2">
         <v>-0.05</v>
       </c>
-      <c r="AH2">
+      <c r="AI2">
         <v>999</v>
       </c>
-      <c r="AI2">
+      <c r="AJ2">
         <v>-999</v>
       </c>
-      <c r="AJ2">
+      <c r="AK2">
         <v>0.02</v>
-      </c>
-      <c r="AK2">
-        <v>10</v>
       </c>
       <c r="AL2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:38">
+      <c r="AM2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>210</v>
+        <v>239</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>210</v>
+        <v>239</v>
       </c>
       <c r="E3" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="H3" t="s">
-        <v>99</v>
+        <v>129</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -3035,102 +3442,105 @@
         <v>0</v>
       </c>
       <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
         <v>0.02</v>
       </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
       <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
         <v>0.1</v>
       </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
       <c r="P3">
         <v>1</v>
       </c>
       <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
         <v>0.8</v>
       </c>
-      <c r="T3">
-        <v>1</v>
-      </c>
       <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3">
         <v>999</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>-999</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>-0.02</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>0.02</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>999</v>
       </c>
-      <c r="Z3">
+      <c r="AA3">
         <v>-999</v>
       </c>
-      <c r="AA3">
-        <v>1</v>
-      </c>
       <c r="AB3">
+        <v>1</v>
+      </c>
+      <c r="AC3">
         <v>0.1</v>
       </c>
-      <c r="AC3">
+      <c r="AD3">
         <v>0.02</v>
       </c>
-      <c r="AD3">
+      <c r="AE3">
         <v>-0.01</v>
       </c>
-      <c r="AE3">
+      <c r="AF3">
         <v>0.01</v>
       </c>
-      <c r="AF3">
+      <c r="AG3">
         <v>0.05</v>
       </c>
-      <c r="AG3">
+      <c r="AH3">
         <v>-0.05</v>
       </c>
-      <c r="AH3">
+      <c r="AI3">
         <v>999</v>
       </c>
-      <c r="AI3">
+      <c r="AJ3">
         <v>-999</v>
       </c>
-      <c r="AJ3">
+      <c r="AK3">
         <v>0.02</v>
-      </c>
-      <c r="AK3">
-        <v>10</v>
       </c>
       <c r="AL3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:38">
+      <c r="AM3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>211</v>
+        <v>240</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>211</v>
+        <v>240</v>
       </c>
       <c r="E4" t="s">
-        <v>178</v>
+        <v>206</v>
       </c>
       <c r="F4" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="H4" t="s">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -3142,102 +3552,105 @@
         <v>0</v>
       </c>
       <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
         <v>0.02</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
       <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
         <v>0.1</v>
       </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
       <c r="P4">
         <v>1</v>
       </c>
       <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
         <v>0.8</v>
       </c>
-      <c r="T4">
-        <v>1</v>
-      </c>
       <c r="U4">
+        <v>1</v>
+      </c>
+      <c r="V4">
         <v>999</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>-999</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>-0.02</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>0.02</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>999</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>-999</v>
       </c>
-      <c r="AA4">
-        <v>1</v>
-      </c>
       <c r="AB4">
+        <v>1</v>
+      </c>
+      <c r="AC4">
         <v>0.1</v>
       </c>
-      <c r="AC4">
+      <c r="AD4">
         <v>0.02</v>
       </c>
-      <c r="AD4">
+      <c r="AE4">
         <v>-0.01</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <v>0.01</v>
       </c>
-      <c r="AF4">
+      <c r="AG4">
         <v>0.05</v>
       </c>
-      <c r="AG4">
+      <c r="AH4">
         <v>-0.05</v>
       </c>
-      <c r="AH4">
+      <c r="AI4">
         <v>999</v>
       </c>
-      <c r="AI4">
+      <c r="AJ4">
         <v>-999</v>
       </c>
-      <c r="AJ4">
+      <c r="AK4">
         <v>0.02</v>
-      </c>
-      <c r="AK4">
-        <v>10</v>
       </c>
       <c r="AL4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:38">
+      <c r="AM4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>241</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>212</v>
+        <v>241</v>
       </c>
       <c r="E5" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>101</v>
+        <v>131</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -3249,102 +3662,105 @@
         <v>0</v>
       </c>
       <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
         <v>0.02</v>
       </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
       <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
         <v>0.1</v>
       </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
       <c r="P5">
         <v>1</v>
       </c>
       <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
         <v>0.8</v>
       </c>
-      <c r="T5">
-        <v>1</v>
-      </c>
       <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
         <v>999</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>-999</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>-0.02</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>0.02</v>
       </c>
-      <c r="Y5">
+      <c r="Z5">
         <v>999</v>
       </c>
-      <c r="Z5">
+      <c r="AA5">
         <v>-999</v>
       </c>
-      <c r="AA5">
-        <v>1</v>
-      </c>
       <c r="AB5">
+        <v>1</v>
+      </c>
+      <c r="AC5">
         <v>0.1</v>
       </c>
-      <c r="AC5">
+      <c r="AD5">
         <v>0.02</v>
       </c>
-      <c r="AD5">
+      <c r="AE5">
         <v>-0.01</v>
       </c>
-      <c r="AE5">
+      <c r="AF5">
         <v>0.01</v>
       </c>
-      <c r="AF5">
+      <c r="AG5">
         <v>0.05</v>
       </c>
-      <c r="AG5">
+      <c r="AH5">
         <v>-0.05</v>
       </c>
-      <c r="AH5">
+      <c r="AI5">
         <v>999</v>
       </c>
-      <c r="AI5">
+      <c r="AJ5">
         <v>-999</v>
       </c>
-      <c r="AJ5">
+      <c r="AK5">
         <v>0.02</v>
-      </c>
-      <c r="AK5">
-        <v>10</v>
       </c>
       <c r="AL5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:38">
+      <c r="AM5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>213</v>
+        <v>242</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>213</v>
+        <v>242</v>
       </c>
       <c r="E6" t="s">
-        <v>180</v>
+        <v>208</v>
       </c>
       <c r="F6" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="H6" t="s">
-        <v>102</v>
+        <v>132</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -3356,78 +3772,81 @@
         <v>0</v>
       </c>
       <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
         <v>0.02</v>
       </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
       <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
         <v>0.1</v>
       </c>
-      <c r="O6">
-        <v>1</v>
-      </c>
       <c r="P6">
         <v>1</v>
       </c>
       <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
         <v>0.8</v>
       </c>
-      <c r="T6">
-        <v>1</v>
-      </c>
       <c r="U6">
+        <v>1</v>
+      </c>
+      <c r="V6">
         <v>999</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>-999</v>
       </c>
-      <c r="W6">
+      <c r="X6">
         <v>-0.02</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>0.02</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <v>999</v>
       </c>
-      <c r="Z6">
+      <c r="AA6">
         <v>-999</v>
       </c>
-      <c r="AA6">
-        <v>1</v>
-      </c>
       <c r="AB6">
+        <v>1</v>
+      </c>
+      <c r="AC6">
         <v>0.1</v>
       </c>
-      <c r="AC6">
+      <c r="AD6">
         <v>0.02</v>
       </c>
-      <c r="AD6">
+      <c r="AE6">
         <v>-0.01</v>
       </c>
-      <c r="AE6">
+      <c r="AF6">
         <v>0.01</v>
       </c>
-      <c r="AF6">
+      <c r="AG6">
         <v>0.05</v>
       </c>
-      <c r="AG6">
+      <c r="AH6">
         <v>-0.05</v>
       </c>
-      <c r="AH6">
+      <c r="AI6">
         <v>999</v>
       </c>
-      <c r="AI6">
+      <c r="AJ6">
         <v>-999</v>
       </c>
-      <c r="AJ6">
+      <c r="AK6">
         <v>0.02</v>
       </c>
-      <c r="AK6">
+      <c r="AL6">
         <v>10</v>
       </c>
-      <c r="AL6">
+      <c r="AM6">
         <v>10</v>
       </c>
     </row>
@@ -3436,7 +3855,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K6"/>
   <sheetViews>
@@ -3449,37 +3868,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>181</v>
+        <v>209</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>59</v>
+        <v>243</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>214</v>
+        <v>244</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>215</v>
+        <v>245</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>216</v>
+        <v>246</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>217</v>
+        <v>247</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>218</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -3487,25 +3906,25 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>219</v>
+        <v>249</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>219</v>
+        <v>249</v>
       </c>
       <c r="E2" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
       <c r="F2">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -3522,25 +3941,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>250</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>220</v>
+        <v>250</v>
       </c>
       <c r="E3" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
       <c r="F3">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -3557,25 +3976,25 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>221</v>
+        <v>251</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>221</v>
+        <v>251</v>
       </c>
       <c r="E4" t="s">
-        <v>178</v>
+        <v>206</v>
       </c>
       <c r="F4">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -3592,25 +4011,25 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="E5" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
       <c r="F5">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="G5">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -3627,25 +4046,25 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>223</v>
+        <v>253</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>223</v>
+        <v>253</v>
       </c>
       <c r="E6" t="s">
-        <v>180</v>
+        <v>208</v>
       </c>
       <c r="F6">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -3662,7 +4081,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -3675,25 +4094,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>224</v>
+        <v>254</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>225</v>
+        <v>255</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>226</v>
+        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -3701,16 +4120,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>227</v>
+        <v>257</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>227</v>
+        <v>257</v>
       </c>
       <c r="E2" t="s">
-        <v>219</v>
+        <v>249</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -3724,16 +4143,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>228</v>
+        <v>258</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>228</v>
+        <v>258</v>
       </c>
       <c r="E3" t="s">
-        <v>220</v>
+        <v>250</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -3747,16 +4166,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>229</v>
+        <v>259</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>229</v>
+        <v>259</v>
       </c>
       <c r="E4" t="s">
-        <v>221</v>
+        <v>251</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -3770,16 +4189,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>230</v>
+        <v>260</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>230</v>
+        <v>260</v>
       </c>
       <c r="E5" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -3793,16 +4212,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>231</v>
+        <v>261</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>231</v>
+        <v>261</v>
       </c>
       <c r="E6" t="s">
-        <v>223</v>
+        <v>253</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -3816,7 +4235,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O6"/>
   <sheetViews>
@@ -3829,49 +4248,49 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>232</v>
+        <v>262</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>233</v>
+        <v>263</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>234</v>
+        <v>264</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>235</v>
+        <v>265</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>236</v>
+        <v>266</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>237</v>
+        <v>267</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>238</v>
+        <v>268</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>239</v>
+        <v>269</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>240</v>
+        <v>270</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>241</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -3879,16 +4298,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>242</v>
+        <v>272</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>242</v>
+        <v>272</v>
       </c>
       <c r="E2" t="s">
-        <v>227</v>
+        <v>257</v>
       </c>
       <c r="F2">
         <v>0.1</v>
@@ -3926,16 +4345,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>243</v>
+        <v>273</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>243</v>
+        <v>273</v>
       </c>
       <c r="E3" t="s">
-        <v>228</v>
+        <v>258</v>
       </c>
       <c r="F3">
         <v>0.1</v>
@@ -3973,16 +4392,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>244</v>
+        <v>274</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>244</v>
+        <v>274</v>
       </c>
       <c r="E4" t="s">
-        <v>229</v>
+        <v>259</v>
       </c>
       <c r="F4">
         <v>0.1</v>
@@ -4020,16 +4439,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>245</v>
+        <v>275</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>245</v>
+        <v>275</v>
       </c>
       <c r="E5" t="s">
-        <v>230</v>
+        <v>260</v>
       </c>
       <c r="F5">
         <v>0.1</v>
@@ -4067,16 +4486,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>246</v>
+        <v>276</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>246</v>
+        <v>276</v>
       </c>
       <c r="E6" t="s">
-        <v>231</v>
+        <v>261</v>
       </c>
       <c r="F6">
         <v>0.1</v>
@@ -4114,9 +4533,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4125,83 +4544,86 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>247</v>
+        <v>277</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>248</v>
+        <v>278</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>249</v>
+        <v>279</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>250</v>
+        <v>280</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>251</v>
+        <v>281</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>252</v>
+        <v>282</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>253</v>
+        <v>283</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>254</v>
+        <v>284</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>255</v>
+        <v>285</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>256</v>
+        <v>286</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>257</v>
+        <v>287</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>258</v>
+        <v>288</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>259</v>
+        <v>289</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>260</v>
+        <v>290</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
+        <v>291</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>262</v>
+        <v>293</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>262</v>
+        <v>293</v>
       </c>
       <c r="E2" t="s">
-        <v>242</v>
+        <v>272</v>
       </c>
       <c r="F2">
         <v>0.1</v>
@@ -4249,21 +4671,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:21">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>263</v>
+        <v>294</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>263</v>
+        <v>294</v>
       </c>
       <c r="E3" t="s">
-        <v>243</v>
+        <v>273</v>
       </c>
       <c r="F3">
         <v>0.1</v>
@@ -4311,21 +4733,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:21">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>264</v>
+        <v>295</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>264</v>
+        <v>295</v>
       </c>
       <c r="E4" t="s">
-        <v>244</v>
+        <v>274</v>
       </c>
       <c r="F4">
         <v>0.1</v>
@@ -4373,21 +4795,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:21">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>265</v>
+        <v>296</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>265</v>
+        <v>296</v>
       </c>
       <c r="E5" t="s">
-        <v>245</v>
+        <v>275</v>
       </c>
       <c r="F5">
         <v>0.1</v>
@@ -4435,21 +4857,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:21">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>266</v>
+        <v>297</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>266</v>
+        <v>297</v>
       </c>
       <c r="E6" t="s">
-        <v>246</v>
+        <v>276</v>
       </c>
       <c r="F6">
         <v>0.1</v>
@@ -4503,6 +4925,91 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3">
+        <v>1.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N15"/>
   <sheetViews>
@@ -4515,46 +5022,46 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -4568,7 +5075,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="E2">
         <v>69</v>
@@ -4612,7 +5119,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="E3">
         <v>69</v>
@@ -4656,7 +5163,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E4">
         <v>69</v>
@@ -4700,7 +5207,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E5">
         <v>69</v>
@@ -4744,7 +5251,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E6">
         <v>69</v>
@@ -4788,7 +5295,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E7">
         <v>138</v>
@@ -4832,7 +5339,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="E8">
         <v>138</v>
@@ -4876,7 +5383,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="E9">
         <v>69</v>
@@ -4920,7 +5427,7 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="E10">
         <v>138</v>
@@ -4964,7 +5471,7 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="E11">
         <v>138</v>
@@ -5008,7 +5515,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E12">
         <v>138</v>
@@ -5052,7 +5559,7 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="E13">
         <v>138</v>
@@ -5096,7 +5603,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E14">
         <v>138</v>
@@ -5140,7 +5647,7 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="E15">
         <v>138</v>
@@ -5178,7 +5685,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K12"/>
   <sheetViews>
@@ -5191,37 +5698,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -5229,13 +5736,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -5264,13 +5771,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -5299,13 +5806,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -5334,13 +5841,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="E5">
         <v>5</v>
@@ -5369,13 +5876,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="E6">
         <v>6</v>
@@ -5404,13 +5911,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="E7">
         <v>9</v>
@@ -5439,13 +5946,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="E8">
         <v>10</v>
@@ -5474,13 +5981,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E9">
         <v>11</v>
@@ -5509,13 +6016,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="E10">
         <v>12</v>
@@ -5544,13 +6051,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="E11">
         <v>13</v>
@@ -5579,13 +6086,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="E12">
         <v>14</v>
@@ -5614,7 +6121,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S5"/>
   <sheetViews>
@@ -5627,61 +6134,61 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -5913,7 +6420,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T2"/>
   <sheetViews>
@@ -5926,64 +6433,64 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -6050,7 +6557,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -6063,34 +6570,34 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -6098,13 +6605,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="E2">
         <v>9</v>
@@ -6130,13 +6637,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="E3">
         <v>14</v>
@@ -6162,7 +6669,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X21"/>
   <sheetViews>
@@ -6175,76 +6682,76 @@
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:24">
@@ -6252,13 +6759,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -6317,13 +6824,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -6382,13 +6889,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -6447,13 +6954,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -6512,13 +7019,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -6577,13 +7084,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -6642,13 +7149,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="E8">
         <v>4</v>
@@ -6707,13 +7214,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="E9">
         <v>6</v>
@@ -6772,13 +7279,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="E10">
         <v>6</v>
@@ -6837,13 +7344,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="E11">
         <v>6</v>
@@ -6902,13 +7409,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="E12">
         <v>7</v>
@@ -6967,13 +7474,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="E13">
         <v>9</v>
@@ -7032,13 +7539,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="E14">
         <v>9</v>
@@ -7097,13 +7604,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="E15">
         <v>10</v>
@@ -7162,13 +7669,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="E16">
         <v>12</v>
@@ -7227,13 +7734,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="E17">
         <v>13</v>
@@ -7292,13 +7799,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="E18">
         <v>4</v>
@@ -7357,13 +7864,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="E19">
         <v>4</v>
@@ -7422,13 +7929,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="E20">
         <v>6</v>
@@ -7487,13 +7994,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="E21">
         <v>8</v>
@@ -7552,7 +8059,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -7565,16 +8072,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -7588,7 +8095,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -7602,179 +8109,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E2">
-        <v>8</v>
-      </c>
-      <c r="F2">
-        <v>0.02</v>
-      </c>
-      <c r="G2">
-        <v>0.02</v>
-      </c>
-      <c r="H2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
-      <c r="F3">
-        <v>0.02</v>
-      </c>
-      <c r="G3">
-        <v>0.02</v>
-      </c>
-      <c r="H3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>0.02</v>
-      </c>
-      <c r="G4">
-        <v>0.02</v>
-      </c>
-      <c r="H4">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>101</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>0.02</v>
-      </c>
-      <c r="G5">
-        <v>0.02</v>
-      </c>
-      <c r="H5">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0.02</v>
-      </c>
-      <c r="G6">
-        <v>0.02</v>
-      </c>
-      <c r="H6">
-        <v>60</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>